<commit_message>
Update Firmware with correct Numpad Keycodes
</commit_message>
<xml_diff>
--- a/bom/teensyNumPadBOM.xlsx
+++ b/bom/teensyNumPadBOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TeensyNumPad\TeensyNumPad\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ABFA07-DD56-40C7-99CB-E1F9B3708DDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84522087-7672-4FD9-AB06-6F53C4AC4570}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44175" yWindow="2535" windowWidth="31455" windowHeight="17445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1575" yWindow="1170" windowWidth="31455" windowHeight="17445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mouser" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Sourced</t>
   </si>
@@ -59,9 +59,6 @@
     <t>603-CFR-25JT-52-150R</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9</t>
-  </si>
-  <si>
     <t xml:space="preserve"> R_Axial_DIN0207_L6.3mm_D2.5mm_P7.62mm_Horizontal</t>
   </si>
   <si>
@@ -86,18 +83,9 @@
     <t>40P_2Row_Pitch2.54 mm</t>
   </si>
   <si>
-    <t>Pin Headers</t>
-  </si>
-  <si>
-    <t>20P_1Row_Pitch2.54 mm</t>
-  </si>
-  <si>
     <t>78-TLHK42T1U2</t>
   </si>
   <si>
-    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
@@ -150,6 +138,15 @@
   </si>
   <si>
     <t>Cut in half</t>
+  </si>
+  <si>
+    <t>R1 - R9</t>
+  </si>
+  <si>
+    <t>LED1 - LED9</t>
+  </si>
+  <si>
+    <t>540-MX1A-11NW</t>
   </si>
 </sst>
 </file>
@@ -300,7 +297,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -376,6 +373,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
@@ -394,158 +399,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
         </patternFill>
       </fill>
     </dxf>
@@ -787,11 +640,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -805,7 +658,7 @@
     <col min="7" max="7" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -828,7 +681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -840,13 +693,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1">
         <v>150</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -856,13 +709,13 @@
         <v>18</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>9</v>
@@ -875,13 +728,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>9</v>
@@ -894,27 +747,29 @@
         <v>1</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8">
-        <v>2</v>
-      </c>
-      <c r="D6" s="15"/>
+        <v>9</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="16" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>21</v>
@@ -927,29 +782,29 @@
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>27</v>
@@ -961,94 +816,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="containsText" dxfId="33" priority="15" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH(("x"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="containsBlanks" dxfId="32" priority="16">
+    <cfRule type="containsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="x">
-      <formula>NOT(ISERROR(SEARCH(("x"),(A9))))</formula>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH(("x"),(A8))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH(("x"),(A4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsBlanks" dxfId="28" priority="14">
+    <cfRule type="containsBlanks" dxfId="11" priority="14">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH(("x"),(A5))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="containsBlanks" dxfId="26" priority="12">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
       <formula>LEN(TRIM(A5))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="containsBlanks" dxfId="24" priority="2">
-      <formula>LEN(TRIM(A9))=0</formula>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="containsBlanks" dxfId="8" priority="2">
+      <formula>LEN(TRIM(A8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH(("x"),(A6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="containsBlanks" dxfId="22" priority="8">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH(("x"),(A7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="containsBlanks" dxfId="20" priority="6">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(A7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="x">
-      <formula>NOT(ISERROR(SEARCH(("x"),(A8))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="containsBlanks" dxfId="18" priority="4">
-      <formula>LEN(TRIM(A8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1079,7 +905,7 @@
     <col min="7" max="7" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>4</v>
@@ -1102,7 +928,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -1114,16 +940,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1131,29 +957,29 @@
         <v>1</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A2">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="1" priority="13" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH(("x"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A2">
-    <cfRule type="containsBlanks" dxfId="12" priority="14">
+    <cfRule type="containsBlanks" dxfId="0" priority="14">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>